<commit_message>
Datasets about HDI and urbanization of the countries uploaded and concatened to the final dataset
</commit_message>
<xml_diff>
--- a/Datasets/Country-List.xlsx
+++ b/Datasets/Country-List.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RodolfoSaldanha/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RodolfoSaldanha/Desktop/IP/final_project/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488B82FC-A9DA-0D49-B523-56EDE64DC73A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24E4C86-4A70-A84A-8E12-469FA5062DDA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="153">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -849,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="F136" sqref="F136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1925,8 +1925,8 @@
       <c r="A132" t="s">
         <v>131</v>
       </c>
-      <c r="C132" t="s">
-        <v>151</v>
+      <c r="C132">
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>